<commit_message>
second commit, added readme, modified mainScript a bit
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Documents\-projects\project-15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0FC301-0FD2-4EBB-A405-3BDC6A44C7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E6597D-8130-490B-AC30-C6B5C76480B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ticker_Code</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>153.75</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>AMZN</t>
   </si>
 </sst>
 </file>
@@ -355,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -383,16 +377,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>